<commit_message>
Optimized NJ algo and nice print visuals
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="11">
   <si>
     <t>Tr1</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Allele</t>
+  </si>
+  <si>
+    <t>39copy</t>
+  </si>
+  <si>
+    <t>weird1</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,18 +597,18 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>129</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -612,46 +619,46 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>92</v>
+        <v>651</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>105</v>
+        <v>651</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>808</v>
+        <v>795</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -659,119 +666,251 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31">
         <v>795</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>14196</v>
-      </c>
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>14196</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>14196</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>14196</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>14196</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>14206</v>
-      </c>
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>14206</v>
+        <v>14196</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>150</v>
+        <v>490</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>14206</v>
+        <v>14196</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>92</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>14206</v>
+        <v>14196</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>627</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
+        <v>14196</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>14196</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>14206</v>
       </c>
-      <c r="B35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35">
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>14206</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>14206</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>14206</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>14206</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47">
         <v>651</v>
       </c>
     </row>

</xml_diff>